<commit_message>
add california to read me
</commit_message>
<xml_diff>
--- a/california_property_price_vs_nq100.xlsx
+++ b/california_property_price_vs_nq100.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -56,208 +59,208 @@
     <t>property_x_5_leverage_return</t>
   </si>
   <si>
+    <t>2024-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1994-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1993-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1993-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1993-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1993-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1992-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1992-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1992-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1992-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1991-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2021-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1991-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2021-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1991-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2021-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1991-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1990-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1990-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1990-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1990-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2019-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1989-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2019-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1989-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2019-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1989-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2019-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1989-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2018-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1988-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2018-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1988-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2018-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1988-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2018-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1988-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2017-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1987-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2017-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1987-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2017-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1987-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2017-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1987-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2016-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1986-10-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2016-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1986-07-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2016-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1986-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2016-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1986-01-01 00:00:00</t>
+  </si>
+  <si>
     <t>2015-10-01 00:00:00</t>
   </si>
   <si>
     <t>1985-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2016-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1986-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2016-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1986-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2016-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1986-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2016-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1986-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1987-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1987-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1987-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1987-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1988-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1988-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1988-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1988-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2019-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1989-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2019-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1989-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2019-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1989-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2019-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1989-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2020-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1990-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2020-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1990-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2020-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1990-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2020-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1990-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2021-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1991-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2021-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1991-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2021-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1991-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2021-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1991-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1992-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1992-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1992-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1992-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2023-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1993-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2023-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1993-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2023-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1993-07-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2023-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1993-10-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2024-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>1994-01-01 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -431,12 +434,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -770,7 +785,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -794,16 +809,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -812,100 +827,100 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1054,106 +1069,106 @@
               <c:strCache>
                 <c:ptCount val="34"/>
                 <c:pt idx="0" c:formatCode="m/d/yyyy;@">
+                  <c:v>2024-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
                   <c:v>2015-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
-                  <c:v>2024-01-01 00:00:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1165,106 +1180,106 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>40.2096846073646</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.4287303870408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.2807498580791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.3567996074308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.7361505904691</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.6126441005307</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.7694796128553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.6237500498542</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43.7549622644657</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.7463983116367</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.3052609857232</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.5369145357057</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.9459383965647</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.681875062571</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43.7754495091895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.652012434148</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41.9069619820938</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.4739248372918</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36.4821386943909</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38.2020969799108</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.1330170871159</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39.4469881924716</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>38.2095914667993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>36.770439980781</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42.148780701084</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.2843370590429</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29.3316335508688</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.4728608725766</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.7878032688985</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33.4035550727026</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.078205394793</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.0226253912887</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31.4863299868923</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>37.8447405465608</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31.4863299868923</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>28.0226253912887</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30.078205394793</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33.4035550727026</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.7878032688985</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28.4728608725766</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29.3316335508688</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>31.2843370590429</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42.148780701084</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>36.770439980781</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>38.2095914667993</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39.4469881924716</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>36.1330170871159</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>38.2020969799108</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>36.4821386943909</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>33.4739248372918</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41.9069619820938</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>39.652012434148</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43.7754495091895</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>65.681875062571</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>61.9459383965647</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>49.5369145357057</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>55.3052609857232</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>51.7463983116367</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43.7549622644657</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43.6237500498542</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>38.7694796128553</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>34.6126441005307</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.7361505904691</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>37.3567996074308</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>42.2807498580791</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>37.4287303870408</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>40.2096846073646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,106 +1321,106 @@
               <c:strCache>
                 <c:ptCount val="34"/>
                 <c:pt idx="0" c:formatCode="m/d/yyyy;@">
+                  <c:v>2024-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
                   <c:v>2015-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
-                  <c:v>2024-01-01 00:00:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1417,106 +1432,106 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>3.44410391814796</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.34332399626517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.30657137553369</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.20457368978052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0652342502623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.01450707388278</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.07688542825361</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.09347661974333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.81489782465392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.64607650273224</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.52963713228818</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.35502906464682</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.14749004332793</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.06068162926018</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.97887874837027</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.96932112021738</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.94521391197292</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.95357635643388</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.02690418254442</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.16837453256277</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.29075159235669</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.4226809622873</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.61029535864979</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.73419362441812</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.81515337423313</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.88863448451313</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.94173424012556</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.98624038850668</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.00096745214567</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.06145013820965</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.11078844199216</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.11106989167532</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.11705989110708</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>3.11643048640368</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.11705989110708</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.11106989167532</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.11078844199216</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.06145013820965</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.00096745214567</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.98624038850668</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.94173424012556</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.88863448451313</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.81515337423313</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.73419362441812</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.61029535864979</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.4226809622873</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.29075159235669</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.16837453256277</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.02690418254442</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.95357635643388</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.94521391197292</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.96932112021738</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.97887874837027</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.06068162926018</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.14749004332793</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.35502906464682</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.52963713228818</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.64607650273224</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.81489782465392</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.09347661974333</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.07688542825361</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.01450707388278</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.0652342502623</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.20457368978052</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.30657137553369</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.34332399626517</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.44410391814796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1558,106 +1573,106 @@
               <c:strCache>
                 <c:ptCount val="34"/>
                 <c:pt idx="0" c:formatCode="m/d/yyyy;@">
+                  <c:v>2024-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
+                  <c:v>2023-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
+                  <c:v>2022-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
+                  <c:v>2021-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
+                  <c:v>2020-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
+                  <c:v>2019-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
+                  <c:v>2018-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
+                  <c:v>2017-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-10-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-07-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-04-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
+                  <c:v>2016-01-01 00:00:00</c:v>
+                </c:pt>
+                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
                   <c:v>2015-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="m/d/yyyy;@">
-                  <c:v>2016-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="m/d/yyyy;@">
-                  <c:v>2017-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="m/d/yyyy;@">
-                  <c:v>2018-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="m/d/yyyy;@">
-                  <c:v>2019-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="m/d/yyyy;@">
-                  <c:v>2020-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="24" c:formatCode="m/d/yyyy;@">
-                  <c:v>2021-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="25" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="26" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="27" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="28" c:formatCode="m/d/yyyy;@">
-                  <c:v>2022-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="29" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-01-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="30" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-04-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="31" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-07-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="32" c:formatCode="m/d/yyyy;@">
-                  <c:v>2023-10-01 00:00:00</c:v>
-                </c:pt>
-                <c:pt idx="33" c:formatCode="m/d/yyyy;@">
-                  <c:v>2024-01-01 00:00:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1669,106 +1684,106 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>21.2205195907398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.7166199813259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.5328568776685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0228684489026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.3261712513115</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.0725353694139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.3844271412681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.4673830987166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.0744891232696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.2303825136612</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.6481856614409</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.7751453232341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.7374502166397</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.3034081463009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.8943937418514</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.8466056010869</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.7260695598646</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.7678817821694</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.1345209127221</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.8418726628139</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.4537579617834</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16.1134048114365</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.0514767932489</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17.6709681220906</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.0757668711656</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18.4431724225657</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.7086712006278</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18.9312019425334</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19.0048372607284</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.3072506910483</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19.5539422099608</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.5553494583766</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19.5852994555354</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>19.5821524320184</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19.5852994555354</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.5553494583766</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19.5539422099608</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.3072506910483</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.0048372607284</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18.9312019425334</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.7086712006278</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.4431724225657</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>18.0757668711656</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17.6709681220906</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17.0514767932489</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.1134048114365</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15.4537579617834</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.8418726628139</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14.1345209127221</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.7678817821694</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13.7260695598646</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>13.8466056010869</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>13.8943937418514</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>14.3034081463009</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14.7374502166397</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15.7751453232341</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>16.6481856614409</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>17.2303825136612</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>18.0744891232696</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>19.4673830987166</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>19.3844271412681</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>19.0725353694139</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>19.3261712513115</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>20.0228684489026</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>20.5328568776685</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>20.7166199813259</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>21.2205195907398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2517,14 +2532,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>225425</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>40005</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2532,8 +2547,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2968625" y="1311275"/>
-        <a:ext cx="7491730" cy="4277995"/>
+        <a:off x="2968625" y="3249930"/>
+        <a:ext cx="7625080" cy="4277995"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2833,8 +2848,8 @@
   <sheetPr/>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2843,8 +2858,8 @@
     <col min="2" max="2" width="21.5714285714286" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.7142857142857" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.7142857142857" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.8571428571429" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.8571428571429" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.8571428571429" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.5714285714286" style="3" customWidth="1"/>
     <col min="9" max="9" width="30.8571428571429" style="3" customWidth="1"/>
@@ -2887,25 +2902,25 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>537.4</v>
+        <v>942.55</v>
       </c>
       <c r="D2" s="2">
-        <v>130.55</v>
+        <v>212.09</v>
       </c>
       <c r="E2" s="2">
-        <v>4415.8701171875</v>
+        <v>16832.919921875</v>
       </c>
       <c r="F2" s="2">
-        <v>113.680000305176</v>
+        <v>408.470001220703</v>
       </c>
       <c r="G2" s="3">
-        <v>37.8447405465608</v>
+        <v>40.2096846073646</v>
       </c>
       <c r="H2" s="3">
-        <v>3.11643048640368</v>
+        <v>3.44410391814796</v>
       </c>
       <c r="I2" s="3">
-        <v>19.5821524320184</v>
+        <v>21.2205195907398</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2916,25 +2931,25 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>544.44</v>
+        <v>930.34</v>
       </c>
       <c r="D3" s="2">
-        <v>132.24</v>
+        <v>214.2</v>
       </c>
       <c r="E3" s="2">
-        <v>4259.77001953125</v>
+        <v>14779.6899414062</v>
       </c>
       <c r="F3" s="2">
-        <v>131.125</v>
+        <v>384.600006103516</v>
       </c>
       <c r="G3" s="3">
-        <v>31.4863299868923</v>
+        <v>37.4287303870408</v>
       </c>
       <c r="H3" s="3">
-        <v>3.11705989110708</v>
+        <v>3.34332399626517</v>
       </c>
       <c r="I3" s="3">
-        <v>19.5852994555354</v>
+        <v>20.7166199813259</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2945,25 +2960,25 @@
         <v>14</v>
       </c>
       <c r="C4" s="2">
-        <v>554.09</v>
+        <v>927.98</v>
       </c>
       <c r="D4" s="2">
-        <v>134.78</v>
+        <v>215.48</v>
       </c>
       <c r="E4" s="2">
-        <v>4496.0400390625</v>
+        <v>15465.509765625</v>
       </c>
       <c r="F4" s="2">
-        <v>154.915000915527</v>
+        <v>357.329986572266</v>
       </c>
       <c r="G4" s="3">
-        <v>28.0226253912887</v>
+        <v>42.2807498580791</v>
       </c>
       <c r="H4" s="3">
-        <v>3.11106989167532</v>
+        <v>3.30657137553369</v>
       </c>
       <c r="I4" s="3">
-        <v>19.5553494583766</v>
+        <v>20.5328568776685</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2974,25 +2989,25 @@
         <v>16</v>
       </c>
       <c r="C5" s="2">
-        <v>566.22</v>
+        <v>913.78</v>
       </c>
       <c r="D5" s="2">
-        <v>137.74</v>
+        <v>217.33</v>
       </c>
       <c r="E5" s="2">
-        <v>4599.88500976563</v>
+        <v>13062.599609375</v>
       </c>
       <c r="F5" s="2">
-        <v>148.009994506836</v>
+        <v>340.554992675781</v>
       </c>
       <c r="G5" s="3">
-        <v>30.078205394793</v>
+        <v>37.3567996074308</v>
       </c>
       <c r="H5" s="3">
-        <v>3.11078844199216</v>
+        <v>3.20457368978052</v>
       </c>
       <c r="I5" s="3">
-        <v>19.5539422099608</v>
+        <v>20.0228684489026</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3003,25 +3018,25 @@
         <v>18</v>
       </c>
       <c r="C6" s="2">
-        <v>573.03</v>
+        <v>891.14</v>
       </c>
       <c r="D6" s="2">
-        <v>141.09</v>
+        <v>219.21</v>
       </c>
       <c r="E6" s="2">
-        <v>4839.72021484375</v>
+        <v>11500.5454101562</v>
       </c>
       <c r="F6" s="2">
-        <v>140.675003051758</v>
+        <v>374.169998168945</v>
       </c>
       <c r="G6" s="3">
-        <v>33.4035550727026</v>
+        <v>29.7361505904691</v>
       </c>
       <c r="H6" s="3">
-        <v>3.06145013820965</v>
+        <v>3.0652342502623</v>
       </c>
       <c r="I6" s="3">
-        <v>19.3072506910483</v>
+        <v>19.3261712513115</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3032,25 +3047,25 @@
         <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>578.98</v>
+        <v>893.83</v>
       </c>
       <c r="D7" s="2">
-        <v>144.71</v>
+        <v>222.65</v>
       </c>
       <c r="E7" s="2">
-        <v>5053.51000976563</v>
+        <v>11191.6298828125</v>
       </c>
       <c r="F7" s="2">
-        <v>164.139999389648</v>
+        <v>314.260009765625</v>
       </c>
       <c r="G7" s="3">
-        <v>29.7878032688985</v>
+        <v>34.6126441005307</v>
       </c>
       <c r="H7" s="3">
-        <v>3.00096745214567</v>
+        <v>3.01450707388278</v>
       </c>
       <c r="I7" s="3">
-        <v>19.0048372607284</v>
+        <v>19.0725353694139</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3061,25 +3076,25 @@
         <v>22</v>
       </c>
       <c r="C8" s="2">
-        <v>591</v>
+        <v>916.28</v>
       </c>
       <c r="D8" s="2">
-        <v>148.26</v>
+        <v>224.75</v>
       </c>
       <c r="E8" s="2">
-        <v>5421.68017578125</v>
+        <v>12097.9750976562</v>
       </c>
       <c r="F8" s="2">
-        <v>183.955001831055</v>
+        <v>304.202499389648</v>
       </c>
       <c r="G8" s="3">
-        <v>28.4728608725766</v>
+        <v>38.7694796128553</v>
       </c>
       <c r="H8" s="3">
-        <v>2.98624038850668</v>
+        <v>3.07688542825361</v>
       </c>
       <c r="I8" s="3">
-        <v>18.9312019425334</v>
+        <v>19.3844271412681</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3090,25 +3105,25 @@
         <v>24</v>
       </c>
       <c r="C9" s="2">
-        <v>602.77</v>
+        <v>921.81</v>
       </c>
       <c r="D9" s="2">
-        <v>152.92</v>
+        <v>225.19</v>
       </c>
       <c r="E9" s="2">
-        <v>5859.92016601563</v>
+        <v>13965.2250976562</v>
       </c>
       <c r="F9" s="2">
-        <v>193.195007324219</v>
+        <v>312.954986572266</v>
       </c>
       <c r="G9" s="3">
-        <v>29.3316335508688</v>
+        <v>43.6237500498542</v>
       </c>
       <c r="H9" s="3">
-        <v>2.94173424012556</v>
+        <v>3.09347661974333</v>
       </c>
       <c r="I9" s="3">
-        <v>18.7086712006278</v>
+        <v>19.4673830987166</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3119,25 +3134,25 @@
         <v>26</v>
       </c>
       <c r="C10" s="2">
-        <v>611.41</v>
+        <v>868.08</v>
       </c>
       <c r="D10" s="2">
-        <v>157.23</v>
+        <v>227.55</v>
       </c>
       <c r="E10" s="2">
-        <v>6075.10522460938</v>
+        <v>15353.1899414062</v>
       </c>
       <c r="F10" s="2">
-        <v>188.175003051758</v>
+        <v>343.050003051758</v>
       </c>
       <c r="G10" s="3">
-        <v>31.2843370590429</v>
+        <v>43.7549622644657</v>
       </c>
       <c r="H10" s="3">
-        <v>2.88863448451313</v>
+        <v>2.81489782465392</v>
       </c>
       <c r="I10" s="3">
-        <v>18.4431724225657</v>
+        <v>18.0744891232696</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3148,25 +3163,25 @@
         <v>28</v>
       </c>
       <c r="C11" s="2">
-        <v>621.87</v>
+        <v>834.04</v>
       </c>
       <c r="D11" s="2">
-        <v>163</v>
+        <v>228.75</v>
       </c>
       <c r="E11" s="2">
-        <v>6810.27978515625</v>
+        <v>15146.919921875</v>
       </c>
       <c r="F11" s="2">
-        <v>157.832496643066</v>
+        <v>287.165008544922</v>
       </c>
       <c r="G11" s="3">
-        <v>42.148780701084</v>
+        <v>51.7463983116367</v>
       </c>
       <c r="H11" s="3">
-        <v>2.81515337423313</v>
+        <v>2.64607650273224</v>
       </c>
       <c r="I11" s="3">
-        <v>18.0757668711656</v>
+        <v>17.2303825136612</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3177,25 +3192,25 @@
         <v>30</v>
       </c>
       <c r="C12" s="2">
-        <v>633.73</v>
+        <v>801.51</v>
       </c>
       <c r="D12" s="2">
-        <v>169.71</v>
+        <v>227.08</v>
       </c>
       <c r="E12" s="2">
-        <v>6615.8701171875</v>
+        <v>14842.6298828125</v>
       </c>
       <c r="F12" s="2">
-        <v>175.159996032715</v>
+        <v>263.610000610352</v>
       </c>
       <c r="G12" s="3">
-        <v>36.770439980781</v>
+        <v>55.3052609857232</v>
       </c>
       <c r="H12" s="3">
-        <v>2.73419362441812</v>
+        <v>2.52963713228818</v>
       </c>
       <c r="I12" s="3">
-        <v>17.6709681220906</v>
+        <v>16.6481856614409</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3206,25 +3221,25 @@
         <v>32</v>
       </c>
       <c r="C13" s="2">
-        <v>641.73</v>
+        <v>761.86</v>
       </c>
       <c r="D13" s="2">
-        <v>177.75</v>
+        <v>227.08</v>
       </c>
       <c r="E13" s="2">
-        <v>7350.22998046875</v>
+        <v>13860.759765625</v>
       </c>
       <c r="F13" s="2">
-        <v>187.459999084473</v>
+        <v>274.270004272461</v>
       </c>
       <c r="G13" s="3">
-        <v>38.2095914667993</v>
+        <v>49.5369145357057</v>
       </c>
       <c r="H13" s="3">
-        <v>2.61029535864979</v>
+        <v>2.35502906464682</v>
       </c>
       <c r="I13" s="3">
-        <v>17.0514767932489</v>
+        <v>15.7751453232341</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3235,25 +3250,25 @@
         <v>34</v>
       </c>
       <c r="C14" s="2">
-        <v>641.65</v>
+        <v>719.17</v>
       </c>
       <c r="D14" s="2">
-        <v>187.47</v>
+        <v>228.49</v>
       </c>
       <c r="E14" s="2">
-        <v>7118.669921875</v>
+        <v>12973.6298828125</v>
       </c>
       <c r="F14" s="2">
-        <v>176</v>
+        <v>206.107498168945</v>
       </c>
       <c r="G14" s="3">
-        <v>39.4469881924716</v>
+        <v>61.9459383965647</v>
       </c>
       <c r="H14" s="3">
-        <v>2.4226809622873</v>
+        <v>2.14749004332793</v>
       </c>
       <c r="I14" s="3">
-        <v>16.1134048114365</v>
+        <v>14.7374502166397</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3264,25 +3279,25 @@
         <v>36</v>
       </c>
       <c r="C15" s="2">
-        <v>645.81</v>
+        <v>699.58</v>
       </c>
       <c r="D15" s="2">
-        <v>196.25</v>
+        <v>228.57</v>
       </c>
       <c r="E15" s="2">
-        <v>6646.81005859375</v>
+        <v>11616.6499023437</v>
       </c>
       <c r="F15" s="2">
-        <v>179</v>
+        <v>174.210006713867</v>
       </c>
       <c r="G15" s="3">
-        <v>36.1330170871159</v>
+        <v>65.681875062571</v>
       </c>
       <c r="H15" s="3">
-        <v>2.29075159235669</v>
+        <v>2.06068162926018</v>
       </c>
       <c r="I15" s="3">
-        <v>15.4537579617834</v>
+        <v>14.3034081463009</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3293,25 +3308,25 @@
         <v>38</v>
       </c>
       <c r="C16" s="2">
-        <v>652.4</v>
+        <v>685.44</v>
       </c>
       <c r="D16" s="2">
-        <v>205.91</v>
+        <v>230.1</v>
       </c>
       <c r="E16" s="2">
-        <v>7629.1201171875</v>
+        <v>10664.8403320312</v>
       </c>
       <c r="F16" s="2">
-        <v>194.610000610352</v>
+        <v>238.184997558594</v>
       </c>
       <c r="G16" s="3">
-        <v>38.2020969799108</v>
+        <v>43.7754495091895</v>
       </c>
       <c r="H16" s="3">
-        <v>2.16837453256277</v>
+        <v>1.97887874837027</v>
       </c>
       <c r="I16" s="3">
-        <v>14.8418726628139</v>
+        <v>13.8943937418514</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3322,25 +3337,25 @@
         <v>40</v>
       </c>
       <c r="C17" s="2">
-        <v>659.29</v>
+        <v>677.51</v>
       </c>
       <c r="D17" s="2">
-        <v>217.81</v>
+        <v>228.17</v>
       </c>
       <c r="E17" s="2">
-        <v>7903.76489257813</v>
+        <v>8641.5</v>
       </c>
       <c r="F17" s="2">
-        <v>210.867500305176</v>
+        <v>212.57250213623</v>
       </c>
       <c r="G17" s="3">
-        <v>36.4821386943909</v>
+        <v>39.652012434148</v>
       </c>
       <c r="H17" s="3">
-        <v>2.02690418254442</v>
+        <v>1.96932112021738</v>
       </c>
       <c r="I17" s="3">
-        <v>14.1345209127221</v>
+        <v>13.8466056010869</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -3351,25 +3366,25 @@
         <v>42</v>
       </c>
       <c r="C18" s="2">
-        <v>663.58</v>
+        <v>669.83</v>
       </c>
       <c r="D18" s="2">
-        <v>224.67</v>
+        <v>227.43</v>
       </c>
       <c r="E18" s="2">
-        <v>7874.6201171875</v>
+        <v>9035.669921875</v>
       </c>
       <c r="F18" s="2">
-        <v>228.422500610352</v>
+        <v>210.587501525879</v>
       </c>
       <c r="G18" s="3">
-        <v>33.4739248372918</v>
+        <v>41.9069619820938</v>
       </c>
       <c r="H18" s="3">
-        <v>1.95357635643388</v>
+        <v>1.94521391197292</v>
       </c>
       <c r="I18" s="3">
-        <v>13.7678817821694</v>
+        <v>13.7260695598646</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3380,25 +3395,25 @@
         <v>44</v>
       </c>
       <c r="C19" s="2">
-        <v>669.83</v>
+        <v>663.58</v>
       </c>
       <c r="D19" s="2">
-        <v>227.43</v>
+        <v>224.67</v>
       </c>
       <c r="E19" s="2">
-        <v>9035.669921875</v>
+        <v>7874.6201171875</v>
       </c>
       <c r="F19" s="2">
-        <v>210.587501525879</v>
+        <v>228.422500610352</v>
       </c>
       <c r="G19" s="3">
-        <v>41.9069619820938</v>
+        <v>33.4739248372918</v>
       </c>
       <c r="H19" s="3">
-        <v>1.94521391197292</v>
+        <v>1.95357635643388</v>
       </c>
       <c r="I19" s="3">
-        <v>13.7260695598646</v>
+        <v>13.7678817821694</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3409,25 +3424,25 @@
         <v>46</v>
       </c>
       <c r="C20" s="2">
-        <v>677.51</v>
+        <v>659.29</v>
       </c>
       <c r="D20" s="2">
-        <v>228.17</v>
+        <v>217.81</v>
       </c>
       <c r="E20" s="2">
-        <v>8641.5</v>
+        <v>7903.76489257813</v>
       </c>
       <c r="F20" s="2">
-        <v>212.57250213623</v>
+        <v>210.867500305176</v>
       </c>
       <c r="G20" s="3">
-        <v>39.652012434148</v>
+        <v>36.4821386943909</v>
       </c>
       <c r="H20" s="3">
-        <v>1.96932112021738</v>
+        <v>2.02690418254442</v>
       </c>
       <c r="I20" s="3">
-        <v>13.8466056010869</v>
+        <v>14.1345209127221</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3438,25 +3453,25 @@
         <v>48</v>
       </c>
       <c r="C21" s="2">
-        <v>685.44</v>
+        <v>652.4</v>
       </c>
       <c r="D21" s="2">
-        <v>230.1</v>
+        <v>205.91</v>
       </c>
       <c r="E21" s="2">
-        <v>10664.8403320312</v>
+        <v>7629.1201171875</v>
       </c>
       <c r="F21" s="2">
-        <v>238.184997558594</v>
+        <v>194.610000610352</v>
       </c>
       <c r="G21" s="3">
-        <v>43.7754495091895</v>
+        <v>38.2020969799108</v>
       </c>
       <c r="H21" s="3">
-        <v>1.97887874837027</v>
+        <v>2.16837453256277</v>
       </c>
       <c r="I21" s="3">
-        <v>13.8943937418514</v>
+        <v>14.8418726628139</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3467,25 +3482,25 @@
         <v>50</v>
       </c>
       <c r="C22" s="2">
-        <v>699.58</v>
+        <v>645.81</v>
       </c>
       <c r="D22" s="2">
-        <v>228.57</v>
+        <v>196.25</v>
       </c>
       <c r="E22" s="2">
-        <v>11616.6499023437</v>
+        <v>6646.81005859375</v>
       </c>
       <c r="F22" s="2">
-        <v>174.210006713867</v>
+        <v>179</v>
       </c>
       <c r="G22" s="3">
-        <v>65.681875062571</v>
+        <v>36.1330170871159</v>
       </c>
       <c r="H22" s="3">
-        <v>2.06068162926018</v>
+        <v>2.29075159235669</v>
       </c>
       <c r="I22" s="3">
-        <v>14.3034081463009</v>
+        <v>15.4537579617834</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3496,25 +3511,25 @@
         <v>52</v>
       </c>
       <c r="C23" s="2">
-        <v>719.17</v>
+        <v>641.65</v>
       </c>
       <c r="D23" s="2">
-        <v>228.49</v>
+        <v>187.47</v>
       </c>
       <c r="E23" s="2">
-        <v>12973.6298828125</v>
+        <v>7118.669921875</v>
       </c>
       <c r="F23" s="2">
-        <v>206.107498168945</v>
+        <v>176</v>
       </c>
       <c r="G23" s="3">
-        <v>61.9459383965647</v>
+        <v>39.4469881924716</v>
       </c>
       <c r="H23" s="3">
-        <v>2.14749004332793</v>
+        <v>2.4226809622873</v>
       </c>
       <c r="I23" s="3">
-        <v>14.7374502166397</v>
+        <v>16.1134048114365</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3525,25 +3540,25 @@
         <v>54</v>
       </c>
       <c r="C24" s="2">
-        <v>761.86</v>
+        <v>641.73</v>
       </c>
       <c r="D24" s="2">
-        <v>227.08</v>
+        <v>177.75</v>
       </c>
       <c r="E24" s="2">
-        <v>13860.759765625</v>
+        <v>7350.22998046875</v>
       </c>
       <c r="F24" s="2">
-        <v>274.270004272461</v>
+        <v>187.459999084473</v>
       </c>
       <c r="G24" s="3">
-        <v>49.5369145357057</v>
+        <v>38.2095914667993</v>
       </c>
       <c r="H24" s="3">
-        <v>2.35502906464682</v>
+        <v>2.61029535864979</v>
       </c>
       <c r="I24" s="3">
-        <v>15.7751453232341</v>
+        <v>17.0514767932489</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3554,25 +3569,25 @@
         <v>56</v>
       </c>
       <c r="C25" s="2">
-        <v>801.51</v>
+        <v>633.73</v>
       </c>
       <c r="D25" s="2">
-        <v>227.08</v>
+        <v>169.71</v>
       </c>
       <c r="E25" s="2">
-        <v>14842.6298828125</v>
+        <v>6615.8701171875</v>
       </c>
       <c r="F25" s="2">
-        <v>263.610000610352</v>
+        <v>175.159996032715</v>
       </c>
       <c r="G25" s="3">
-        <v>55.3052609857232</v>
+        <v>36.770439980781</v>
       </c>
       <c r="H25" s="3">
-        <v>2.52963713228818</v>
+        <v>2.73419362441812</v>
       </c>
       <c r="I25" s="3">
-        <v>16.6481856614409</v>
+        <v>17.6709681220906</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3583,25 +3598,25 @@
         <v>58</v>
       </c>
       <c r="C26" s="2">
-        <v>834.04</v>
+        <v>621.87</v>
       </c>
       <c r="D26" s="2">
-        <v>228.75</v>
+        <v>163</v>
       </c>
       <c r="E26" s="2">
-        <v>15146.919921875</v>
+        <v>6810.27978515625</v>
       </c>
       <c r="F26" s="2">
-        <v>287.165008544922</v>
+        <v>157.832496643066</v>
       </c>
       <c r="G26" s="3">
-        <v>51.7463983116367</v>
+        <v>42.148780701084</v>
       </c>
       <c r="H26" s="3">
-        <v>2.64607650273224</v>
+        <v>2.81515337423313</v>
       </c>
       <c r="I26" s="3">
-        <v>17.2303825136612</v>
+        <v>18.0757668711656</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3612,25 +3627,25 @@
         <v>60</v>
       </c>
       <c r="C27" s="2">
-        <v>868.08</v>
+        <v>611.41</v>
       </c>
       <c r="D27" s="2">
-        <v>227.55</v>
+        <v>157.23</v>
       </c>
       <c r="E27" s="2">
-        <v>15353.1899414062</v>
+        <v>6075.10522460938</v>
       </c>
       <c r="F27" s="2">
-        <v>343.050003051758</v>
+        <v>188.175003051758</v>
       </c>
       <c r="G27" s="3">
-        <v>43.7549622644657</v>
+        <v>31.2843370590429</v>
       </c>
       <c r="H27" s="3">
-        <v>2.81489782465392</v>
+        <v>2.88863448451313</v>
       </c>
       <c r="I27" s="3">
-        <v>18.0744891232696</v>
+        <v>18.4431724225657</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3641,25 +3656,25 @@
         <v>62</v>
       </c>
       <c r="C28" s="2">
-        <v>921.81</v>
+        <v>602.77</v>
       </c>
       <c r="D28" s="2">
-        <v>225.19</v>
+        <v>152.92</v>
       </c>
       <c r="E28" s="2">
-        <v>13965.2250976562</v>
+        <v>5859.92016601563</v>
       </c>
       <c r="F28" s="2">
-        <v>312.954986572266</v>
+        <v>193.195007324219</v>
       </c>
       <c r="G28" s="3">
-        <v>43.6237500498542</v>
+        <v>29.3316335508688</v>
       </c>
       <c r="H28" s="3">
-        <v>3.09347661974333</v>
+        <v>2.94173424012556</v>
       </c>
       <c r="I28" s="3">
-        <v>19.4673830987166</v>
+        <v>18.7086712006278</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -3670,25 +3685,25 @@
         <v>64</v>
       </c>
       <c r="C29" s="2">
-        <v>916.28</v>
+        <v>591</v>
       </c>
       <c r="D29" s="2">
-        <v>224.75</v>
+        <v>148.26</v>
       </c>
       <c r="E29" s="2">
-        <v>12097.9750976562</v>
+        <v>5421.68017578125</v>
       </c>
       <c r="F29" s="2">
-        <v>304.202499389648</v>
+        <v>183.955001831055</v>
       </c>
       <c r="G29" s="3">
-        <v>38.7694796128553</v>
+        <v>28.4728608725766</v>
       </c>
       <c r="H29" s="3">
-        <v>3.07688542825361</v>
+        <v>2.98624038850668</v>
       </c>
       <c r="I29" s="3">
-        <v>19.3844271412681</v>
+        <v>18.9312019425334</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3699,25 +3714,25 @@
         <v>66</v>
       </c>
       <c r="C30" s="2">
-        <v>893.83</v>
+        <v>578.98</v>
       </c>
       <c r="D30" s="2">
-        <v>222.65</v>
+        <v>144.71</v>
       </c>
       <c r="E30" s="2">
-        <v>11191.6298828125</v>
+        <v>5053.51000976563</v>
       </c>
       <c r="F30" s="2">
-        <v>314.260009765625</v>
+        <v>164.139999389648</v>
       </c>
       <c r="G30" s="3">
-        <v>34.6126441005307</v>
+        <v>29.7878032688985</v>
       </c>
       <c r="H30" s="3">
-        <v>3.01450707388278</v>
+        <v>3.00096745214567</v>
       </c>
       <c r="I30" s="3">
-        <v>19.0725353694139</v>
+        <v>19.0048372607284</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3728,25 +3743,25 @@
         <v>68</v>
       </c>
       <c r="C31" s="2">
-        <v>891.14</v>
+        <v>573.03</v>
       </c>
       <c r="D31" s="2">
-        <v>219.21</v>
+        <v>141.09</v>
       </c>
       <c r="E31" s="2">
-        <v>11500.5454101562</v>
+        <v>4839.72021484375</v>
       </c>
       <c r="F31" s="2">
-        <v>374.169998168945</v>
+        <v>140.675003051758</v>
       </c>
       <c r="G31" s="3">
-        <v>29.7361505904691</v>
+        <v>33.4035550727026</v>
       </c>
       <c r="H31" s="3">
-        <v>3.0652342502623</v>
+        <v>3.06145013820965</v>
       </c>
       <c r="I31" s="3">
-        <v>19.3261712513115</v>
+        <v>19.3072506910483</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3757,25 +3772,25 @@
         <v>70</v>
       </c>
       <c r="C32" s="2">
-        <v>913.78</v>
+        <v>566.22</v>
       </c>
       <c r="D32" s="2">
-        <v>217.33</v>
+        <v>137.74</v>
       </c>
       <c r="E32" s="2">
-        <v>13062.599609375</v>
+        <v>4599.88500976563</v>
       </c>
       <c r="F32" s="2">
-        <v>340.554992675781</v>
+        <v>148.009994506836</v>
       </c>
       <c r="G32" s="3">
-        <v>37.3567996074308</v>
+        <v>30.078205394793</v>
       </c>
       <c r="H32" s="3">
-        <v>3.20457368978052</v>
+        <v>3.11078844199216</v>
       </c>
       <c r="I32" s="3">
-        <v>20.0228684489026</v>
+        <v>19.5539422099608</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3786,25 +3801,25 @@
         <v>72</v>
       </c>
       <c r="C33" s="2">
-        <v>927.98</v>
+        <v>554.09</v>
       </c>
       <c r="D33" s="2">
-        <v>215.48</v>
+        <v>134.78</v>
       </c>
       <c r="E33" s="2">
-        <v>15465.509765625</v>
+        <v>4496.0400390625</v>
       </c>
       <c r="F33" s="2">
-        <v>357.329986572266</v>
+        <v>154.915000915527</v>
       </c>
       <c r="G33" s="3">
-        <v>42.2807498580791</v>
+        <v>28.0226253912887</v>
       </c>
       <c r="H33" s="3">
-        <v>3.30657137553369</v>
+        <v>3.11106989167532</v>
       </c>
       <c r="I33" s="3">
-        <v>20.5328568776685</v>
+        <v>19.5553494583766</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3815,25 +3830,25 @@
         <v>74</v>
       </c>
       <c r="C34" s="2">
-        <v>930.34</v>
+        <v>544.44</v>
       </c>
       <c r="D34" s="2">
-        <v>214.2</v>
+        <v>132.24</v>
       </c>
       <c r="E34" s="2">
-        <v>14779.6899414062</v>
+        <v>4259.77001953125</v>
       </c>
       <c r="F34" s="2">
-        <v>384.600006103516</v>
+        <v>131.125</v>
       </c>
       <c r="G34" s="3">
-        <v>37.4287303870408</v>
+        <v>31.4863299868923</v>
       </c>
       <c r="H34" s="3">
-        <v>3.34332399626517</v>
+        <v>3.11705989110708</v>
       </c>
       <c r="I34" s="3">
-        <v>20.7166199813259</v>
+        <v>19.5852994555354</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3844,28 +3859,34 @@
         <v>76</v>
       </c>
       <c r="C35" s="2">
-        <v>942.55</v>
+        <v>537.4</v>
       </c>
       <c r="D35" s="2">
-        <v>212.09</v>
+        <v>130.55</v>
       </c>
       <c r="E35" s="2">
-        <v>16832.919921875</v>
+        <v>4415.8701171875</v>
       </c>
       <c r="F35" s="2">
-        <v>408.470001220703</v>
+        <v>113.680000305176</v>
       </c>
       <c r="G35" s="3">
-        <v>40.2096846073646</v>
+        <v>37.8447405465608</v>
       </c>
       <c r="H35" s="3">
-        <v>3.44410391814796</v>
+        <v>3.11643048640368</v>
       </c>
       <c r="I35" s="3">
-        <v>21.2205195907398</v>
+        <v>19.5821524320184</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I35" etc:filterBottomFollowUsedRange="0">
+    <sortState ref="A2:I35">
+      <sortCondition ref="A2" descending="1"/>
+    </sortState>
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>